<commit_message>
changes done to test case 007
</commit_message>
<xml_diff>
--- a/src/test/java/com/nopcommerce/testData/AddCustomerNew.xlsx
+++ b/src/test/java/com/nopcommerce/testData/AddCustomerNew.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAnsari\eclipse-workspace2022\nopCommerceV1\src\test\java\com\nopcommerce\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAnsari\git\nopCommerceV1\src\test\java\com\nopcommerce\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EB0C8E-65BB-42B0-A97B-4A480AD9B67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D264B64-6730-429D-8686-6EB2A2D7F70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1Bkup" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="88">
   <si>
     <t>CustomerEmail</t>
   </si>
@@ -288,6 +290,9 @@
   </si>
   <si>
     <t>New Customer has been added to the company 100</t>
+  </si>
+  <si>
+    <t>testsssssss1@xyz.com</t>
   </si>
 </sst>
 </file>
@@ -635,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,402 +806,579 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2">
-        <v>38545</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" t="s">
-        <v>61</v>
-      </c>
-      <c r="O4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="2">
-        <v>38546</v>
-      </c>
-      <c r="I5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2">
-        <v>38547</v>
-      </c>
-      <c r="I6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" t="s">
-        <v>63</v>
-      </c>
-      <c r="N6" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="2">
-        <v>38548</v>
-      </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2">
-        <v>38549</v>
-      </c>
-      <c r="I8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" t="s">
-        <v>61</v>
-      </c>
-      <c r="O8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="2">
-        <v>38550</v>
-      </c>
-      <c r="I9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2">
-        <v>38551</v>
-      </c>
-      <c r="I10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" t="s">
-        <v>63</v>
-      </c>
-      <c r="N10" t="s">
-        <v>61</v>
-      </c>
-      <c r="O10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="2">
-        <v>38552</v>
-      </c>
-      <c r="I11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" t="s">
-        <v>73</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{65C03B56-A410-4CDB-80A7-35F704F519E1}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{0CC325F7-1B38-4494-ACFE-5F0DBD2E70FF}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{C96981A1-D175-4775-9F0A-4043B4E8C9F9}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{D894E624-6185-44B5-A4C9-EB541D3656DE}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{57BEE2D0-FC0D-4763-B7B3-F5193DC677E2}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{29ECE70A-A5B1-46EF-9D4C-83AC54655446}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{03C9D47B-0959-4C4B-BBFE-3DDC1CC04227}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{96E2031C-28D0-4D24-BD21-92E05AFF1B30}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{F9A1266F-C97C-49D2-B2BE-8FC853FA7F4D}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{38E5327F-2EA9-4C1D-81E8-8722A79F6CBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA2A799-C99F-4CBB-8E5F-98CD642B2371}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
+        <v>38543</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2">
+        <v>38544</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2">
+        <v>38545</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2">
+        <v>38546</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2">
+        <v>38547</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2">
+        <v>38548</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2">
+        <v>38549</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2">
+        <v>38550</v>
+      </c>
+      <c r="I9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2">
+        <v>38551</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N10" t="s">
+        <v>61</v>
+      </c>
+      <c r="O10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="2">
+        <v>38552</v>
+      </c>
+      <c r="I11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7D8C90DE-9244-48BC-86DC-7151DCF527EF}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{2ACC135C-4FEF-4E76-8165-A25C649E947D}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{E40E58F4-6A62-49BA-A3F5-4809662D91A3}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{B2CC2313-F9EA-4C6E-B78C-1E8052A314CE}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{4C2C7112-EB90-4873-B4B0-9E5D6812AD91}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{A17BF605-3F35-470C-B115-A6F788FF938C}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{2619B3DB-A683-4059-96D2-76FF048F1F7B}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{DB8E84B4-BDB1-498D-B5CF-C9825FA96A9D}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{F6E85D56-C1BE-4D4E-B97A-CED31CAB0882}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{97208BA8-5FDD-4935-9787-EBA431E1FC8C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02AD9CF-A9E8-4BC7-9C4B-FE8F1AA7B46F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1247,17 +1429,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAE67EB-C0BB-4B5C-9CE3-0BF1B2AFE2FA}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="4"/>
     <col min="3" max="3" width="31.44140625" style="4" customWidth="1"/>
     <col min="4" max="16384" width="11.5546875" style="4"/>
   </cols>
@@ -1290,4 +1473,47 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892E39E2-D2E5-427D-8080-0C10D3EC4A35}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2DA10655-2778-482E-841E-54AF1E2D751D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>